<commit_message>
Add one new test case on Page Product assert
</commit_message>
<xml_diff>
--- a/bin/dataEngine/DataEngine.xlsx
+++ b/bin/dataEngine/DataEngine.xlsx
@@ -4,19 +4,19 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" firstSheet="1" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="001_LoginCorrectly" sheetId="2" r:id="rId1"/>
     <sheet name="002_LoginIncorrectly" sheetId="1" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="004_AccessoriesPage" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="25">
   <si>
     <t>TestCase</t>
   </si>
@@ -46,6 +46,51 @@
   </si>
   <si>
     <t>O42Ds8vvBlO</t>
+  </si>
+  <si>
+    <t>004-Test Accessories Page</t>
+  </si>
+  <si>
+    <t>Product Name</t>
+  </si>
+  <si>
+    <t>Magic Mouse</t>
+  </si>
+  <si>
+    <t>Apple TV</t>
+  </si>
+  <si>
+    <t>Sennheiser RS 120</t>
+  </si>
+  <si>
+    <t>Skullcandy PLYR 1 – Black</t>
+  </si>
+  <si>
+    <t>Apple 27 inch Thunderbolt Display</t>
+  </si>
+  <si>
+    <t>Asus MX239H 23-inch Widescreen AH</t>
+  </si>
+  <si>
+    <t>Product Prices</t>
+  </si>
+  <si>
+    <t>$150.00</t>
+  </si>
+  <si>
+    <t>$80.00</t>
+  </si>
+  <si>
+    <t>$50.00</t>
+  </si>
+  <si>
+    <t>$110.00</t>
+  </si>
+  <si>
+    <t>$764.00</t>
+  </si>
+  <si>
+    <t>$199.00</t>
   </si>
 </sst>
 </file>
@@ -81,8 +126,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -386,8 +432,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -440,7 +486,7 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+      <selection sqref="A1:C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -491,12 +537,83 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="22.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.77734375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.5546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Finish all the test case about product browse
</commit_message>
<xml_diff>
--- a/bin/dataEngine/DataEngine.xlsx
+++ b/bin/dataEngine/DataEngine.xlsx
@@ -4,19 +4,24 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" firstSheet="1" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" firstSheet="6" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="001_LoginCorrectly" sheetId="2" r:id="rId1"/>
     <sheet name="002_LoginIncorrectly" sheetId="1" r:id="rId2"/>
     <sheet name="004_AccessoriesPage" sheetId="3" r:id="rId3"/>
+    <sheet name="005_iMacsPage" sheetId="4" r:id="rId4"/>
+    <sheet name="006_iPadsPage" sheetId="5" r:id="rId5"/>
+    <sheet name="007_iPhonesPage" sheetId="6" r:id="rId6"/>
+    <sheet name="008_iPodsPage" sheetId="7" r:id="rId7"/>
+    <sheet name="009_MacBooksPage" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="42">
   <si>
     <t>TestCase</t>
   </si>
@@ -91,6 +96,57 @@
   </si>
   <si>
     <t>$199.00</t>
+  </si>
+  <si>
+    <t>005-Test iMacs Page</t>
+  </si>
+  <si>
+    <t>Apple iPad 2 16GB, Wi-Fi, 9.7in – Black</t>
+  </si>
+  <si>
+    <t>$270.00</t>
+  </si>
+  <si>
+    <t>Apple iPad 6 32GB (White, 3D)</t>
+  </si>
+  <si>
+    <t>$680.00</t>
+  </si>
+  <si>
+    <t>006-Test iPads Page</t>
+  </si>
+  <si>
+    <t>007-Test iPhones Page</t>
+  </si>
+  <si>
+    <t>Apple iPhone 4S 16GB SIM-Free – Black</t>
+  </si>
+  <si>
+    <t>Apple iPhone 4S 32GB SIM-Free – White</t>
+  </si>
+  <si>
+    <t>Apple iPod touch 32GB 5th Generation – Black</t>
+  </si>
+  <si>
+    <t>$204.00</t>
+  </si>
+  <si>
+    <t>Apple iPod touch Large</t>
+  </si>
+  <si>
+    <t>$10.00</t>
+  </si>
+  <si>
+    <t>Apple 13-inch MacBook Pro</t>
+  </si>
+  <si>
+    <t>$864.00</t>
+  </si>
+  <si>
+    <t>008-Test iPods Page</t>
+  </si>
+  <si>
+    <t>009-Test MacBooks Page</t>
   </si>
 </sst>
 </file>
@@ -539,8 +595,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -616,4 +672,270 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="17.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.5546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="17.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.5546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="19.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="33.21875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.5546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="19.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="39.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.5546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="21.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.77734375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.5546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>